<commit_message>
small non ideal tracing update
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorrit/Documents/master-software-engineering/thesis/DYNAMOS/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0503D2-1B50-114D-8479-F0ED53A9AB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950CE0AF-A00A-4242-840F-09912DD3C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5120" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
   </bookViews>
@@ -375,9 +375,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,11 +933,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1074,7 +1074,7 @@
   <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,13 +1099,13 @@
       <c r="A4">
         <v>10000</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>1344567</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>1179764</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>983455</v>
       </c>
     </row>
@@ -1113,13 +1113,13 @@
       <c r="A5">
         <v>30000</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>4036427</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>3542478</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>2955314</v>
       </c>
     </row>

</xml_diff>

<commit_message>
slightly improved tracing, should convert to openT
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorrit/Documents/master-software-engineering/thesis/DYNAMOS/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950CE0AF-A00A-4242-840F-09912DD3C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC00728-8870-D149-B906-8616D311CC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
+    <workbookView xWindow="2100" yWindow="1940" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservices" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="134">
   <si>
     <t>Receive messages from an input queue</t>
   </si>
@@ -290,20 +290,164 @@
     <t>After processing, return results to data analyst</t>
   </si>
   <si>
-    <t>proto</t>
-  </si>
-  <si>
-    <t>Json</t>
-  </si>
-  <si>
-    <t>disk</t>
+    <t>TraceID</t>
+  </si>
+  <si>
+    <t>Archetype</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>JSON string</t>
+  </si>
+  <si>
+    <t>JSON bytes</t>
+  </si>
+  <si>
+    <t>proto-wire format</t>
+  </si>
+  <si>
+    <t>disk (bytes)</t>
+  </si>
+  <si>
+    <t>Seconds to write to file</t>
+  </si>
+  <si>
+    <t>0.021</t>
+  </si>
+  <si>
+    <t>0.055</t>
+  </si>
+  <si>
+    <t>0.117</t>
+  </si>
+  <si>
+    <t>0.168</t>
+  </si>
+  <si>
+    <t>DataThroughTtp</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>11.9</t>
+  </si>
+  <si>
+    <t>b0aa7091c839796822260a12a8920d50</t>
+  </si>
+  <si>
+    <t>3.14</t>
+  </si>
+  <si>
+    <t>62f38f06b7826e166d875ecc7944e3ab</t>
+  </si>
+  <si>
+    <t>3.19</t>
+  </si>
+  <si>
+    <t>bbb3b105566e7b0051c933bf806e82e3</t>
+  </si>
+  <si>
+    <t>3.86</t>
+  </si>
+  <si>
+    <t>3d2a0d7bd5204cd7a54bdddc3416d745</t>
+  </si>
+  <si>
+    <t>2.98</t>
+  </si>
+  <si>
+    <t>c0bac2379cfe4b7edbc8ca66530379a5</t>
+  </si>
+  <si>
+    <t>2.99</t>
+  </si>
+  <si>
+    <t>59b56d872e4fc86b276a42eaf16b66a9</t>
+  </si>
+  <si>
+    <t>6.84</t>
+  </si>
+  <si>
+    <t>1495941eda9f4127d17349bc98999bd9</t>
+  </si>
+  <si>
+    <t>6.77</t>
+  </si>
+  <si>
+    <t>ee70d6511929dcc13825bda4ea273852</t>
+  </si>
+  <si>
+    <t>5.28</t>
+  </si>
+  <si>
+    <t>0abf854cab71b78a00d54333fe497f93</t>
+  </si>
+  <si>
+    <t>5.42</t>
+  </si>
+  <si>
+    <t>12aeab211e56f7dda68fcc2da95ad091</t>
+  </si>
+  <si>
+    <t>5.09</t>
+  </si>
+  <si>
+    <t>9c93032c8e7ce5a2f2fb93beb36d6cf8</t>
+  </si>
+  <si>
+    <t>ea634f31089539e7a7ff62a4ae74ff4b</t>
+  </si>
+  <si>
+    <t>10.7</t>
+  </si>
+  <si>
+    <t>94ca493d38d2f001c51c071e7f81a6fe</t>
+  </si>
+  <si>
+    <t>7.77</t>
+  </si>
+  <si>
+    <t>e5be6bba30dce2e3e57c619ca44832c2</t>
+  </si>
+  <si>
+    <t>7.31</t>
+  </si>
+  <si>
+    <t>6f6eb7ec6e99897fb4551f79a7969d35</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>7e34cdb0b7a0dbe5d04266a3f1362464</t>
+  </si>
+  <si>
+    <t>11.7</t>
+  </si>
+  <si>
+    <t>f9ce4c7d15493f24bfe4e410a803275b</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>9ade36b4d5bddbfdfdbc01737a9337a9</t>
+  </si>
+  <si>
+    <t>6ab6d2440e14a880a917ad190e21af54</t>
+  </si>
+  <si>
+    <t>10.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +488,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,10 +514,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -375,11 +528,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -933,11 +1099,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1071,59 +1237,532 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E058B4D8-EEB6-994D-9F38-3AD51C0357E5}">
-  <dimension ref="A2:D5"/>
+  <dimension ref="B9:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D9" s="9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="10">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="E10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11">
+        <v>14973</v>
+      </c>
+      <c r="I10" s="11">
+        <v>13647</v>
+      </c>
+      <c r="J10" s="11">
+        <v>307</v>
+      </c>
+      <c r="K10" s="11">
+        <v>9986</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="10">
+        <v>100</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="10">
+        <v>100</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="10">
+        <v>100</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="10">
+        <v>100</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="10">
         <v>10000</v>
       </c>
-      <c r="B4" s="7">
-        <v>1344567</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1179764</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="E16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11">
+        <v>1344899</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1180220</v>
+      </c>
+      <c r="J16" s="11">
+        <v>307</v>
+      </c>
+      <c r="K16" s="11">
         <v>983455</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="L16" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E22" s="10">
+        <v>10</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11">
+        <v>2693365</v>
+      </c>
+      <c r="I22" s="11">
+        <v>2364465</v>
+      </c>
+      <c r="J22" s="11">
+        <v>307</v>
+      </c>
+      <c r="K22" s="11">
+        <v>2463677</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="10">
         <v>30000</v>
       </c>
-      <c r="B5" s="7">
-        <v>4036427</v>
-      </c>
-      <c r="C5" s="7">
-        <v>3542478</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="E28" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="11">
+        <v>4036759</v>
+      </c>
+      <c r="I28" s="11">
+        <v>3542934</v>
+      </c>
+      <c r="J28" s="11">
+        <v>307</v>
+      </c>
+      <c r="K28" s="11">
         <v>2955314</v>
       </c>
+      <c r="L28" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="10">
+        <v>30000</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="10">
+        <v>30000</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="10">
+        <v>30000</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="13"/>
+      <c r="C32" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="10">
+        <v>30000</v>
+      </c>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="10"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" tooltip="Trace: b0aa7091c839796822260a12a8920d50" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22b0aa7091c839796822260a12a8920d50%22%7D%5D%7D" xr:uid="{FA862687-D425-5244-A318-080B25310B8D}"/>
+    <hyperlink ref="B11" r:id="rId2" tooltip="Trace: 62f38f06b7826e166d875ecc7944e3ab" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%2262f38f06b7826e166d875ecc7944e3ab%22%7D%5D%7D" xr:uid="{D560CD0F-740B-6D4B-8F05-3CEA4CE3C6C1}"/>
+    <hyperlink ref="B12" r:id="rId3" tooltip="Trace: bbb3b105566e7b0051c933bf806e82e3" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22bbb3b105566e7b0051c933bf806e82e3%22%7D%5D%7D" xr:uid="{C2EB725E-B7DE-3E46-9AAE-8A3622C16999}"/>
+    <hyperlink ref="B13" r:id="rId4" tooltip="Trace: 3d2a0d7bd5204cd7a54bdddc3416d745" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%223d2a0d7bd5204cd7a54bdddc3416d745%22%7D%5D%7D" xr:uid="{FD207D8E-A912-104C-9AD0-88C142DEBA05}"/>
+    <hyperlink ref="B16" r:id="rId5" tooltip="Trace: 59b56d872e4fc86b276a42eaf16b66a9" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%2259b56d872e4fc86b276a42eaf16b66a9%22%7D%5D%7D" xr:uid="{DA551EAD-26A6-114E-A527-E568858E61AE}"/>
+    <hyperlink ref="B17" r:id="rId6" tooltip="Trace: 1495941eda9f4127d17349bc98999bd9" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%221495941eda9f4127d17349bc98999bd9%22%7D%5D%7D" xr:uid="{EB29317C-D4D8-E241-ADD3-AC921A0B7CEB}"/>
+    <hyperlink ref="B18" r:id="rId7" tooltip="Trace: ee70d6511929dcc13825bda4ea273852" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22ee70d6511929dcc13825bda4ea273852%22%7D%5D%7D" xr:uid="{AB201069-4D6B-F142-8FA8-E32F705FACC9}"/>
+    <hyperlink ref="B19" r:id="rId8" tooltip="Trace: 0abf854cab71b78a00d54333fe497f93" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%220abf854cab71b78a00d54333fe497f93%22%7D%5D%7D" xr:uid="{DDB9BE39-BEEF-7440-B2C6-AC0576892B97}"/>
+    <hyperlink ref="B20" r:id="rId9" tooltip="Trace: 12aeab211e56f7dda68fcc2da95ad091" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%2212aeab211e56f7dda68fcc2da95ad091%22%7D%5D%7D" xr:uid="{426AA024-2EBD-8440-B0BF-FE91C03D8648}"/>
+    <hyperlink ref="B22" r:id="rId10" tooltip="Trace: 9c93032c8e7ce5a2f2fb93beb36d6cf8" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%229c93032c8e7ce5a2f2fb93beb36d6cf8%22%7D%5D%7D" xr:uid="{B5BC3DA0-FA28-FF47-8488-8831E44DD075}"/>
+    <hyperlink ref="B23" r:id="rId11" tooltip="Trace: ea634f31089539e7a7ff62a4ae74ff4b" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22ea634f31089539e7a7ff62a4ae74ff4b%22%7D%5D%7D" xr:uid="{04841AC9-B9A3-CF4D-9144-6CE46CA6511D}"/>
+    <hyperlink ref="B24" r:id="rId12" tooltip="Trace: 94ca493d38d2f001c51c071e7f81a6fe" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%2294ca493d38d2f001c51c071e7f81a6fe%22%7D%5D%7D" xr:uid="{57F53D48-84B1-CB4C-A51C-6ABD97F30C3F}"/>
+    <hyperlink ref="B25" r:id="rId13" tooltip="Trace: e5be6bba30dce2e3e57c619ca44832c2" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22e5be6bba30dce2e3e57c619ca44832c2%22%7D%5D%7D" xr:uid="{F0E11DC4-9089-674F-8893-F68986294EB9}"/>
+    <hyperlink ref="B26" r:id="rId14" tooltip="Trace: 6f6eb7ec6e99897fb4551f79a7969d35" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%226f6eb7ec6e99897fb4551f79a7969d35%22%7D%5D%7D" xr:uid="{B7E97498-B31F-034B-8863-E064AC49A007}"/>
+    <hyperlink ref="B28" r:id="rId15" tooltip="Trace: 7e34cdb0b7a0dbe5d04266a3f1362464" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%227e34cdb0b7a0dbe5d04266a3f1362464%22%7D%5D%7D" xr:uid="{AF334414-E124-5741-B3C8-25C65F3E9CB1}"/>
+    <hyperlink ref="B29" r:id="rId16" tooltip="Trace: f9ce4c7d15493f24bfe4e410a803275b" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22f9ce4c7d15493f24bfe4e410a803275b%22%7D%5D%7D" xr:uid="{E099D857-1F81-8D43-B914-F080D0313FA3}"/>
+    <hyperlink ref="B30" r:id="rId17" tooltip="Trace: 9ade36b4d5bddbfdfdbc01737a9337a9" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22bde90582-8a87-45cf-981a-9f5d1777f6f0%22%2C%22queries%22%3A%5B%7B%22query%22%3A%229ade36b4d5bddbfdfdbc01737a9337a9%22%7D%5D%7D" xr:uid="{442E219F-32EF-BB40-A1F8-B2DE7F505124}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
bugfix algorithm, finished measurements
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorrit/Documents/master-software-engineering/thesis/DYNAMOS/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5864A003-B4BD-464C-B1A4-5BBC03434BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812FCB98-2257-984C-B055-3AC3D64098B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1940" windowWidth="31740" windowHeight="17440" activeTab="2" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
+    <workbookView xWindow="17920" yWindow="1580" windowWidth="31740" windowHeight="17440" activeTab="2" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservices" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="163">
   <si>
     <t>Receive messages from an input queue</t>
   </si>
@@ -392,9 +392,6 @@
     <t>4.5</t>
   </si>
   <si>
-    <t>bebfc6fd</t>
-  </si>
-  <si>
     <t>f4e494e3a7607fcee24b4e29d7c26eb3</t>
   </si>
   <si>
@@ -450,6 +447,87 @@
   </si>
   <si>
     <t>8.01</t>
+  </si>
+  <si>
+    <t>4433b19eced5d4739439989288f15f0a</t>
+  </si>
+  <si>
+    <t>3.31</t>
+  </si>
+  <si>
+    <t>cf582a7c1445d40e4815756699f00cef</t>
+  </si>
+  <si>
+    <t>3.43</t>
+  </si>
+  <si>
+    <t>24f5181f8b604a0b328a45a8346ed422</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>3d5de56aee170d75e636a491b2a9d4b0</t>
+  </si>
+  <si>
+    <t>4.12</t>
+  </si>
+  <si>
+    <t>9f8442162985c967d47d4a64f1c8be4a</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>555c7732b118ddae6487c0f7335a3811</t>
+  </si>
+  <si>
+    <t>b7be3ebf9b59c78da1e7465bde376bf0</t>
+  </si>
+  <si>
+    <t>5.08</t>
+  </si>
+  <si>
+    <t>7df306ae8e6ad503b66475c5fcae312e</t>
+  </si>
+  <si>
+    <t>4.85</t>
+  </si>
+  <si>
+    <t>51aee5c2f10794e0c00f9a9affc36be2</t>
+  </si>
+  <si>
+    <t>4.69</t>
+  </si>
+  <si>
+    <t>1f5cf3101001ec2958d87157de9ff05e</t>
+  </si>
+  <si>
+    <t>6.47</t>
+  </si>
+  <si>
+    <t>9b5a3a699733e5cf9fc9ce610030ae3e</t>
+  </si>
+  <si>
+    <t>988b82a173043c9fb255ef6836a13da4</t>
+  </si>
+  <si>
+    <t>f7be89afcdc3892b2bd2e65d5ea0edcb</t>
+  </si>
+  <si>
+    <t>5.59</t>
+  </si>
+  <si>
+    <t>938ef240abfc392dc6ce906e84570887</t>
+  </si>
+  <si>
+    <t>5.89</t>
+  </si>
+  <si>
+    <t>61a026f82c5fd6fbcc2a1672aca7aa15</t>
+  </si>
+  <si>
+    <t>4.74</t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E058B4D8-EEB6-994D-9F38-3AD51C0357E5}">
-  <dimension ref="B5:P42"/>
+  <dimension ref="B8:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1396,11 +1474,6 @@
     <col min="24" max="24" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I5" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>95</v>
@@ -1465,12 +1538,27 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="C10" s="10">
         <v>10000</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="10">
+        <f>16032-15917</f>
+        <v>115</v>
+      </c>
+      <c r="F10" s="10">
+        <f>16159-16060</f>
+        <v>99</v>
+      </c>
+      <c r="G10">
+        <f>16316-16159</f>
+        <v>157</v>
+      </c>
       <c r="I10" s="12" t="s">
         <v>106</v>
       </c>
@@ -1502,12 +1590,27 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="C11" s="10">
         <v>10000</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="10">
+        <f>33806-33710</f>
+        <v>96</v>
+      </c>
+      <c r="F11" s="10">
+        <f>33936-33826</f>
+        <v>110</v>
+      </c>
+      <c r="G11">
+        <f>34096-33936</f>
+        <v>160</v>
+      </c>
       <c r="I11" s="12" t="s">
         <v>109</v>
       </c>
@@ -1539,13 +1642,27 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>161</v>
+      </c>
       <c r="C12" s="10">
         <v>10000</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="10">
+        <f>34295-34183</f>
+        <v>112</v>
+      </c>
+      <c r="F12" s="10">
+        <f>34559-34461</f>
+        <v>98</v>
+      </c>
+      <c r="G12">
+        <f>34703-34559</f>
+        <v>144</v>
+      </c>
       <c r="I12" s="12" t="s">
         <v>111</v>
       </c>
@@ -1577,13 +1694,27 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>140</v>
+      </c>
       <c r="C13" s="10">
         <v>10000</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="10">
+        <f>53636-53539</f>
+        <v>97</v>
+      </c>
+      <c r="F13" s="10">
+        <f>53768-53660</f>
+        <v>108</v>
+      </c>
+      <c r="G13">
+        <f>53967-53768</f>
+        <v>199</v>
+      </c>
       <c r="I13" s="12" t="s">
         <v>113</v>
       </c>
@@ -1615,13 +1746,27 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="12"/>
+      <c r="B14" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="C14" s="10">
         <v>10000</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="10">
+        <f>45372-45259</f>
+        <v>113</v>
+      </c>
+      <c r="F14" s="10">
+        <f>45519-45400</f>
+        <v>119</v>
+      </c>
+      <c r="G14">
+        <f>45694-45519</f>
+        <v>175</v>
+      </c>
       <c r="I14" s="12" t="s">
         <v>115</v>
       </c>
@@ -1668,17 +1813,32 @@
       <c r="P15" s="23"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>144</v>
+      </c>
       <c r="C16" s="10">
         <v>20000</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16">
+        <f>14915-14729</f>
+        <v>186</v>
+      </c>
+      <c r="F16" s="10">
+        <f>15152-14947</f>
+        <v>205</v>
+      </c>
+      <c r="G16">
+        <f>15499-15152</f>
+        <v>347</v>
+      </c>
       <c r="I16" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J16" s="21" t="s">
         <v>118</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>119</v>
       </c>
       <c r="K16" s="22">
         <f>656-465</f>
@@ -1705,15 +1865,29 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="12"/>
+      <c r="B17" s="12" t="s">
+        <v>146</v>
+      </c>
       <c r="C17" s="10">
         <v>20000</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17">
+        <f>26228-26061</f>
+        <v>167</v>
+      </c>
+      <c r="F17" s="10">
+        <f>26515-26259</f>
+        <v>256</v>
+      </c>
+      <c r="G17">
+        <f>26841-26515</f>
+        <v>326</v>
+      </c>
       <c r="I17" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J17" s="21" t="s">
         <v>93</v>
@@ -1742,18 +1916,32 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="12"/>
+      <c r="B18" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="C18" s="10">
         <v>20000</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="10">
+        <f>42879-42539</f>
+        <v>340</v>
+      </c>
+      <c r="F18" s="10">
+        <f>43368-43026</f>
+        <v>342</v>
+      </c>
+      <c r="G18">
+        <f>43707-43368</f>
+        <v>339</v>
+      </c>
       <c r="I18" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="K18" s="22">
         <f>1085-930</f>
@@ -1780,18 +1968,32 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="12"/>
+      <c r="B19" s="12" t="s">
+        <v>149</v>
+      </c>
       <c r="C19" s="10">
         <v>20000</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="10">
+        <f>56432-56251</f>
+        <v>181</v>
+      </c>
+      <c r="F19" s="10">
+        <f>56713-56474</f>
+        <v>239</v>
+      </c>
+      <c r="G19">
+        <f>57062-56713</f>
+        <v>349</v>
+      </c>
       <c r="I19" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J19" s="21" t="s">
         <v>123</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>124</v>
       </c>
       <c r="K19" s="22">
         <f>299-142</f>
@@ -1818,18 +2020,32 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="12"/>
+      <c r="B20" s="12" t="s">
+        <v>151</v>
+      </c>
       <c r="C20" s="10">
         <v>20000</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="10">
+        <f>15159-14968</f>
+        <v>191</v>
+      </c>
+      <c r="F20" s="10">
+        <f>15476-15195</f>
+        <v>281</v>
+      </c>
+      <c r="G20">
+        <f>15815-15476</f>
+        <v>339</v>
+      </c>
       <c r="I20" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J20" s="21" t="s">
         <v>125</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>126</v>
       </c>
       <c r="K20" s="22">
         <f>764-599</f>
@@ -1871,18 +2087,32 @@
       <c r="P21" s="23"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="12"/>
+      <c r="B22" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="C22" s="10">
         <v>30000</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="10">
+        <f>38623-38305</f>
+        <v>318</v>
+      </c>
+      <c r="F22" s="10">
+        <f>39444-38768</f>
+        <v>676</v>
+      </c>
+      <c r="G22">
+        <f>40151-39444</f>
+        <v>707</v>
+      </c>
       <c r="I22" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>128</v>
       </c>
       <c r="K22" s="22">
         <f>18421-18174</f>
@@ -1909,16 +2139,32 @@
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="12"/>
+      <c r="B23" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="C23" s="10">
         <v>30000</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23">
+        <f>58544-58291</f>
+        <v>253</v>
+      </c>
+      <c r="F23">
+        <f>59243-58585</f>
+        <v>658</v>
+      </c>
+      <c r="G23">
+        <f>59743-59243</f>
+        <v>500</v>
+      </c>
       <c r="I23" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>130</v>
       </c>
       <c r="K23" s="22">
         <f>35955-35585</f>
@@ -1945,16 +2191,32 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="12"/>
+      <c r="B24" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="C24" s="10">
         <v>30000</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24">
+        <f>12829-12579</f>
+        <v>250</v>
+      </c>
+      <c r="F24">
+        <f>13386-12888</f>
+        <v>498</v>
+      </c>
+      <c r="G24">
+        <f>13972-13386</f>
+        <v>586</v>
+      </c>
       <c r="I24" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="21" t="s">
         <v>131</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>132</v>
       </c>
       <c r="K24" s="22">
         <f>1067-666</f>
@@ -1981,16 +2243,32 @@
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="12"/>
+      <c r="B25" s="12" t="s">
+        <v>157</v>
+      </c>
       <c r="C25" s="10">
         <v>30000</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25">
+        <f>29479-29210</f>
+        <v>269</v>
+      </c>
+      <c r="F25">
+        <f>30220-29551</f>
+        <v>669</v>
+      </c>
+      <c r="G25">
+        <f>30841-30220</f>
+        <v>621</v>
+      </c>
       <c r="I25" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="21" t="s">
         <v>133</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>134</v>
       </c>
       <c r="K25" s="22">
         <f>15283-15030</f>
@@ -2018,16 +2296,32 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="12"/>
+      <c r="B26" s="12" t="s">
+        <v>159</v>
+      </c>
       <c r="C26" s="10">
         <v>30000</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26">
+        <f>43684-43452</f>
+        <v>232</v>
+      </c>
+      <c r="F26">
+        <f>44048-43733</f>
+        <v>315</v>
+      </c>
+      <c r="G26">
+        <f>44524-44048</f>
+        <v>476</v>
+      </c>
       <c r="I26" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="J26" s="24" t="s">
         <v>135</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>136</v>
       </c>
       <c r="K26" s="25">
         <f>31457-31217</f>
@@ -2213,6 +2507,19 @@
     <hyperlink ref="I24" r:id="rId13" tooltip="Trace: c7bb8be8cb5c585b27de791211148a52" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22c7bb8be8cb5c585b27de791211148a52%22%7D%5D%7D" xr:uid="{1E0A3D41-6DC1-F647-8CE9-A56ED16DEF0F}"/>
     <hyperlink ref="I25" r:id="rId14" tooltip="Trace: 3ff6b1cc4294cfba7c2a2a06ab995cdd" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%223ff6b1cc4294cfba7c2a2a06ab995cdd%22%7D%5D%7D" xr:uid="{68A7FFE1-4779-9E47-AFEC-D9909871537C}"/>
     <hyperlink ref="I26" r:id="rId15" tooltip="Trace: 4bfc4fe9a001ca2b2a5baec9e6a40fb9" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%224bfc4fe9a001ca2b2a5baec9e6a40fb9%22%7D%5D%7D" xr:uid="{B6C09F00-3DD7-474A-B68F-1E3E96AB61D5}"/>
+    <hyperlink ref="B10" r:id="rId16" tooltip="Trace: 4433b19eced5d4739439989288f15f0a" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%224433b19eced5d4739439989288f15f0a%22%7D%5D%7D" xr:uid="{4BB6B610-C03E-A44C-B3D7-893B3A592F02}"/>
+    <hyperlink ref="B11" r:id="rId17" tooltip="Trace: cf582a7c1445d40e4815756699f00cef" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22cf582a7c1445d40e4815756699f00cef%22%7D%5D%7D" xr:uid="{C121BD4B-F158-0A4F-81B1-EC976A27C6AA}"/>
+    <hyperlink ref="B14" r:id="rId18" tooltip="Trace: 3d5de56aee170d75e636a491b2a9d4b0" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%223d5de56aee170d75e636a491b2a9d4b0%22%7D%5D%7D" xr:uid="{62BB0104-1323-6E49-B8AE-F7CAC9977B43}"/>
+    <hyperlink ref="B16" r:id="rId19" tooltip="Trace: 9f8442162985c967d47d4a64f1c8be4a" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%229f8442162985c967d47d4a64f1c8be4a%22%7D%5D%7D" xr:uid="{DE9FE605-BF7E-4C42-BAE3-20D3FA0A17A8}"/>
+    <hyperlink ref="B17" r:id="rId20" tooltip="Trace: 555c7732b118ddae6487c0f7335a3811" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22555c7732b118ddae6487c0f7335a3811%22%7D%5D%7D" xr:uid="{CC9898BD-9097-B942-9DC2-E8BB60F5CD2C}"/>
+    <hyperlink ref="B18" r:id="rId21" tooltip="Trace: b7be3ebf9b59c78da1e7465bde376bf0" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22b7be3ebf9b59c78da1e7465bde376bf0%22%7D%5D%7D" xr:uid="{4A1D1B8D-CF73-254E-B62B-E0792E891022}"/>
+    <hyperlink ref="B19" r:id="rId22" tooltip="Trace: 7df306ae8e6ad503b66475c5fcae312e" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%227df306ae8e6ad503b66475c5fcae312e%22%7D%5D%7D" xr:uid="{9D89EEF3-5195-BB4F-92AB-DB30DA8F95BE}"/>
+    <hyperlink ref="B20" r:id="rId23" tooltip="Trace: 51aee5c2f10794e0c00f9a9affc36be2" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%2251aee5c2f10794e0c00f9a9affc36be2%22%7D%5D%7D" xr:uid="{5F19F994-95E3-EB41-A454-56D74C6BFFC5}"/>
+    <hyperlink ref="B22" r:id="rId24" tooltip="Trace: 1f5cf3101001ec2958d87157de9ff05e" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%221f5cf3101001ec2958d87157de9ff05e%22%7D%5D%7D" xr:uid="{2DEF1C2E-179E-004E-BBEC-E425A0E54ACA}"/>
+    <hyperlink ref="B23" r:id="rId25" tooltip="Trace: 9b5a3a699733e5cf9fc9ce610030ae3e" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%229b5a3a699733e5cf9fc9ce610030ae3e%22%7D%5D%7D" xr:uid="{69D00CAF-F389-FD4B-900B-4CFBAAC60851}"/>
+    <hyperlink ref="B24" r:id="rId26" tooltip="Trace: 988b82a173043c9fb255ef6836a13da4" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22988b82a173043c9fb255ef6836a13da4%22%7D%5D%7D" xr:uid="{5A55AFCB-EF24-D641-B08A-B546E90D767B}"/>
+    <hyperlink ref="B25" r:id="rId27" tooltip="Trace: f7be89afcdc3892b2bd2e65d5ea0edcb" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22f7be89afcdc3892b2bd2e65d5ea0edcb%22%7D%5D%7D" xr:uid="{43F1EF18-EB94-314E-A8CD-63072792D9CF}"/>
+    <hyperlink ref="B26" r:id="rId28" tooltip="Trace: 938ef240abfc392dc6ce906e84570887" display="http://localhost:30001/grafana/explore?left=%7B%22range%22%3A%7B%22from%22%3A%22now-1h%22%2C%22to%22%3A%22now%22%7D%2C%22datasource%22%3A%22PC9A941E8F2E49454%22%2C%22queries%22%3A%5B%7B%22query%22%3A%22938ef240abfc392dc6ce906e84570887%22%7D%5D%7D" xr:uid="{5E263B18-FE6A-BC44-A6D1-9AAD270B6871}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
started job deletion on archetype change
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorrit/Documents/master-software-engineering/thesis/DYNAMOS/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D96A335-99E8-E444-AA6B-CE1F617F4020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBAB684-D142-FA4B-B3BC-166C10110C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="500" windowWidth="32120" windowHeight="20200" activeTab="3" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
+    <workbookView xWindow="4020" yWindow="500" windowWidth="32120" windowHeight="20200" activeTab="3" xr2:uid="{D6BE7BD5-07AA-4048-B7F7-9B37E5199ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Microservices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="226">
   <si>
     <t>Receive messages from an input queue</t>
   </si>
@@ -667,6 +667,57 @@
   </si>
   <si>
     <t>The test took 7m9.01669741s seconds to execute.</t>
+  </si>
+  <si>
+    <t>Name:                artifact-passingxjd42</t>
+  </si>
+  <si>
+    <t>Namespace:           argo</t>
+  </si>
+  <si>
+    <t>ServiceAccount:      unset (will run with the default ServiceAccount)</t>
+  </si>
+  <si>
+    <t>Status:              Succeeded</t>
+  </si>
+  <si>
+    <t>Conditions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PodRunning          False</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Completed           True</t>
+  </si>
+  <si>
+    <t>Created:             Wed Aug 02 14:38:58 +0200 (20 seconds ago)</t>
+  </si>
+  <si>
+    <t>Started:             Wed Aug 02 14:38:58 +0200 (20 seconds ago)</t>
+  </si>
+  <si>
+    <t>Finished:            Wed Aug 02 14:39:18 +0200 (now)</t>
+  </si>
+  <si>
+    <t>Duration:            20 seconds</t>
+  </si>
+  <si>
+    <t>Progress:            2/2</t>
+  </si>
+  <si>
+    <t>ResourcesDuration:   9s*(1 cpu),9s*(100Mi memory)</t>
+  </si>
+  <si>
+    <t>STEP                      TEMPLATE          PODNAME                                         DURATION  MESSAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ artifact-passingxjd42  artifact-example</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ├───✔ generate-artifact  whalesay          artifact-passingxjd42-whalesay-4165260985       5s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> └───✔ consume-artifact   print-message     artifact-passingxjd42-print-message-3486085679  5s</t>
   </si>
 </sst>
 </file>
@@ -3990,10 +4041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D402B211-41A9-054B-9CDE-A7E508CC657A}">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="B91" sqref="B91:B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5413,6 +5464,91 @@
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>